<commit_message>
Update data - Oscillibacter valericigenes
</commit_message>
<xml_diff>
--- a/input/phenotype_microbiome_cat.xlsx
+++ b/input/phenotype_microbiome_cat.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\AppData\Roaming\MobaXterm\slash\RemoteFiles\132688_2_14\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\AppData\Roaming\MobaXterm\slash\RemoteFiles\525916_2_9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D45D146F-D82E-40ED-908E-3D172D89AE11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2EDE961-0655-48A5-9200-B32A66A88A41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="59370" yWindow="420" windowWidth="11175" windowHeight="585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51135" yWindow="2610" windowWidth="22425" windowHeight="585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="5" r:id="rId1"/>
@@ -855,9 +855,6 @@
     <t>s__Oxalobacter_formigenes</t>
   </si>
   <si>
-    <t>Oscillobacter valericigenes</t>
-  </si>
-  <si>
     <t>s__Oscillibacter_valericigenes</t>
   </si>
   <si>
@@ -901,6 +898,10 @@
   </si>
   <si>
     <t>s__Prevotella_copri</t>
+  </si>
+  <si>
+    <t>Oscillibacter valericigenes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1644,8 +1645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8871BB2B-37C0-44CD-B7A8-BCB5971E399A}">
   <dimension ref="A1:E1093"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:E1093"/>
+    <sheetView tabSelected="1" topLeftCell="A214" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G221" sqref="G221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -3133,10 +3134,10 @@
         <v>205</v>
       </c>
       <c r="B99" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="C99" s="10" t="s">
         <v>272</v>
-      </c>
-      <c r="C99" s="10" t="s">
-        <v>273</v>
       </c>
       <c r="D99" s="10"/>
       <c r="E99" s="5" t="s">
@@ -3330,7 +3331,7 @@
         <v>127</v>
       </c>
       <c r="B112" s="37" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C112" s="31" t="s">
         <v>128</v>
@@ -3345,7 +3346,7 @@
         <v>127</v>
       </c>
       <c r="B113" s="37" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C113" s="31" t="s">
         <v>129</v>
@@ -5007,10 +5008,10 @@
         <v>187</v>
       </c>
       <c r="B223" s="51" t="s">
+        <v>274</v>
+      </c>
+      <c r="C223" s="51" t="s">
         <v>259</v>
-      </c>
-      <c r="C223" s="51" t="s">
-        <v>260</v>
       </c>
       <c r="D223" s="4"/>
       <c r="E223" s="57" t="s">
@@ -5022,10 +5023,10 @@
         <v>187</v>
       </c>
       <c r="B224" s="64" t="s">
+        <v>260</v>
+      </c>
+      <c r="C224" s="64" t="s">
         <v>261</v>
-      </c>
-      <c r="C224" s="64" t="s">
-        <v>262</v>
       </c>
       <c r="D224" s="4"/>
       <c r="E224" s="57" t="s">
@@ -5202,10 +5203,10 @@
         <v>187</v>
       </c>
       <c r="B236" s="51" t="s">
+        <v>262</v>
+      </c>
+      <c r="C236" s="51" t="s">
         <v>263</v>
-      </c>
-      <c r="C236" s="51" t="s">
-        <v>264</v>
       </c>
       <c r="D236" s="4"/>
       <c r="E236" s="57" t="s">
@@ -5217,10 +5218,10 @@
         <v>187</v>
       </c>
       <c r="B237" s="54" t="s">
+        <v>264</v>
+      </c>
+      <c r="C237" s="54" t="s">
         <v>265</v>
-      </c>
-      <c r="C237" s="54" t="s">
-        <v>266</v>
       </c>
       <c r="D237" s="10"/>
       <c r="E237" s="62" t="s">
@@ -5550,7 +5551,7 @@
         <v>199</v>
       </c>
       <c r="C259" s="31" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D259" s="31"/>
       <c r="E259" s="32" t="s">
@@ -5652,10 +5653,10 @@
         <v>218</v>
       </c>
       <c r="B266" s="52" t="s">
+        <v>266</v>
+      </c>
+      <c r="C266" s="52" t="s">
         <v>267</v>
-      </c>
-      <c r="C266" s="52" t="s">
-        <v>268</v>
       </c>
       <c r="D266" s="17"/>
       <c r="E266" s="53" t="s">
@@ -5667,10 +5668,10 @@
         <v>218</v>
       </c>
       <c r="B267" s="52" t="s">
+        <v>268</v>
+      </c>
+      <c r="C267" s="52" t="s">
         <v>269</v>
-      </c>
-      <c r="C267" s="52" t="s">
-        <v>270</v>
       </c>
       <c r="D267" s="17"/>
       <c r="E267" s="53" t="s">

</xml_diff>